<commit_message>
Created separate .csv files
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@94188 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/ontology/Gates/SCORE/doc/SCORE_DataPrep.xlsx
+++ b/Load/ontology/Gates/SCORE/doc/SCORE_DataPrep.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13220" yWindow="2900" windowWidth="9930" windowHeight="5900" activeTab="1"/>
+    <workbookView xWindow="13220" yWindow="2900" windowWidth="9930" windowHeight="5900" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="STUDY_AllVariables" sheetId="1" r:id="rId1"/>
-    <sheet name="VariableMapping" sheetId="2" r:id="rId2"/>
-    <sheet name="ValueMapping" sheetId="3" r:id="rId3"/>
+    <sheet name="SCORECrossSect_AllVariables" sheetId="1" r:id="rId1"/>
+    <sheet name="SCORECrossSect_VariableMapping" sheetId="2" r:id="rId2"/>
+    <sheet name="SCORECrossSect_ValueMapping" sheetId="3" r:id="rId3"/>
     <sheet name="Notes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -3026,7 +3026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
@@ -13454,7 +13454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>